<commit_message>
Restructured buildings only view
</commit_message>
<xml_diff>
--- a/BuildingAnalysis.xlsx
+++ b/BuildingAnalysis.xlsx
@@ -1,30 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samsm\source\repos\DSPTree\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5AFF6E8-AF72-46FD-A44C-FD3EC7F8C796}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C55DF95-9544-44FB-ADA6-8CDA532190FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15675" activeTab="2" xr2:uid="{8DF00D36-5A31-4E6A-9ACB-13E2EFC23796}"/>
   </bookViews>
   <sheets>
     <sheet name="Lanes" sheetId="1" r:id="rId1"/>
-    <sheet name="Pivot Table" sheetId="3" r:id="rId2"/>
-    <sheet name="Frequencies" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId2"/>
+    <sheet name="Pivot Table" sheetId="3" r:id="rId3"/>
+    <sheet name="Frequencies" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Frequencies!$A$1:$E$48</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Pivot Table'!$A$1:$A$195</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Frequencies!$A$1:$F$47</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Pivot Table'!$A$1:$A$195</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$A$1:$A$253</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="11" r:id="rId4"/>
+    <pivotCache cacheId="3" r:id="rId5"/>
   </pivotCaches>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -44,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="98">
   <si>
     <t>Building</t>
   </si>
@@ -317,6 +320,27 @@
   </si>
   <si>
     <t>Deuteron Fuel Rod</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>1,2,3</t>
+  </si>
+  <si>
+    <t>1,2</t>
+  </si>
+  <si>
+    <t>2,3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
 </sst>
 </file>
@@ -372,7 +396,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -381,6 +405,8 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -400,7 +426,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Sam Smith" refreshedDate="44624.681223263891" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="157" xr:uid="{0389E4B8-E087-4409-A28D-55DFA4FAA855}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Sam Smith" refreshedDate="44625.316425462966" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="157" xr:uid="{0389E4B8-E087-4409-A28D-55DFA4FAA855}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:A1048576" sheet="Pivot Table"/>
   </cacheSource>
@@ -942,7 +968,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{77EBC6EF-0474-435B-B885-9D5274F36D4D}" name="PivotTable2" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{77EBC6EF-0474-435B-B885-9D5274F36D4D}" name="PivotTable2" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="F3:G51" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="1">
     <pivotField axis="axisRow" dataField="1" showAll="0">
@@ -1464,8 +1490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E562AADC-9189-423D-B12E-A6352B054605}">
   <dimension ref="A2:F51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B49" sqref="B49:D51"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1503,10 +1529,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" t="s">
         <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
@@ -1941,196 +1967,190 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>52</v>
+        <v>85</v>
       </c>
       <c r="B36" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C36" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="D36" t="s">
-        <v>53</v>
+        <v>88</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B37" t="s">
-        <v>55</v>
+        <v>17</v>
       </c>
       <c r="C37" t="s">
         <v>34</v>
       </c>
       <c r="D37" t="s">
-        <v>56</v>
-      </c>
-      <c r="E37" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B38" t="s">
         <v>55</v>
       </c>
       <c r="C38" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="D38" t="s">
+        <v>56</v>
+      </c>
+      <c r="E38" t="s">
         <v>41</v>
-      </c>
-      <c r="E38" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B39" t="s">
-        <v>33</v>
+        <v>55</v>
+      </c>
+      <c r="C39" t="s">
+        <v>23</v>
+      </c>
+      <c r="D39" t="s">
+        <v>41</v>
+      </c>
+      <c r="E39" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B40" t="s">
-        <v>55</v>
-      </c>
-      <c r="C40" t="s">
-        <v>53</v>
-      </c>
-      <c r="D40" t="s">
-        <v>34</v>
-      </c>
-      <c r="E40" t="s">
-        <v>40</v>
-      </c>
-      <c r="F40" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B41" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C41" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D41" t="s">
-        <v>51</v>
+        <v>34</v>
+      </c>
+      <c r="E41" t="s">
+        <v>40</v>
+      </c>
+      <c r="F41" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B42" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="C42" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="D42" t="s">
-        <v>62</v>
-      </c>
-      <c r="E42" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B43" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="C43" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="D43" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="E43" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B44" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="C44" t="s">
-        <v>65</v>
+        <v>4</v>
       </c>
       <c r="D44" t="s">
-        <v>66</v>
+        <v>34</v>
+      </c>
+      <c r="E44" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>67</v>
+        <v>86</v>
       </c>
       <c r="B45" t="s">
-        <v>12</v>
+        <v>55</v>
       </c>
       <c r="C45" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="D45" t="s">
-        <v>68</v>
-      </c>
-      <c r="E45" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B46" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="C46" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="D46" t="s">
-        <v>71</v>
-      </c>
-      <c r="E46" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B47" t="s">
-        <v>55</v>
+        <v>12</v>
       </c>
       <c r="C47" t="s">
         <v>53</v>
       </c>
       <c r="D47" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E47" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B48" t="s">
         <v>55</v>
@@ -2139,55 +2159,61 @@
         <v>53</v>
       </c>
       <c r="D48" t="s">
-        <v>34</v>
+        <v>71</v>
       </c>
       <c r="E48" t="s">
         <v>66</v>
       </c>
-      <c r="F48" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B49" t="s">
-        <v>3</v>
+        <v>89</v>
       </c>
       <c r="C49" t="s">
-        <v>41</v>
+        <v>90</v>
       </c>
       <c r="D49" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="B50" t="s">
         <v>55</v>
       </c>
       <c r="C50" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="D50" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
+        <v>73</v>
+      </c>
+      <c r="E50" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="B51" t="s">
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="C51" t="s">
-        <v>90</v>
+        <v>53</v>
       </c>
       <c r="D51" t="s">
+        <v>34</v>
+      </c>
+      <c r="E51" t="s">
         <v>66</v>
+      </c>
+      <c r="F51" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -2196,11 +2222,819 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43B24A0B-6AE3-4A29-B439-E08C2ACBF3F0}">
+  <dimension ref="A1:A157"/>
+  <sheetViews>
+    <sheetView topLeftCell="A145" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A157"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="22.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A40" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A42" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A43" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A44" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A45" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A46" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A47" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A48" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A49" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A50" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A51" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A52" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A53" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A54" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A55" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A56" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A57" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A58" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A59" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A60" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A61" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A62" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A63" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A64" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A65" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A66" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A67" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A68" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A69" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A70" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A71" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A72" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A73" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A74" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A75" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A76" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A77" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A78" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A79" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A80" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A81" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A82" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A83" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A84" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A85" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A86" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A87" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A88" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A89" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A90" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A91" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A92" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A93" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A94" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A95" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A96" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A97" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A98" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A99" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A100" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A101" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A102" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A103" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A104" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A105" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A106" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A107" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A108" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A109" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A110" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A111" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A112" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A113" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A114" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A115" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A116" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A117" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A118" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A119" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A120" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A121" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A122" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A123" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A124" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A125" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A126" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A127" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A128" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A129" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A130" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A131" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A132" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A133" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A134" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A135" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A136" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A137" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A138" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A139" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A140" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A141" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A142" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A143" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A144" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A145" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A146" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A147" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A148" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A149" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A150" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A151" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A152" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A153" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A154" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A155" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A156" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A157" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:A253" xr:uid="{43B24A0B-6AE3-4A29-B439-E08C2ACBF3F0}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A253">
+      <sortCondition ref="A1:A253"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26DD2DF2-8C76-4608-A3EA-012E788C06A7}">
   <dimension ref="A1:G157"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3299,12 +4133,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC4DB84E-5142-48A4-9DBD-FEBC42E0B80D}">
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3314,9 +4148,10 @@
     <col min="3" max="3" width="5.59765625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.19921875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.06640625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
         <v>80</v>
       </c>
@@ -3332,8 +4167,11 @@
       <c r="E1" s="5" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F1" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3341,11 +4179,14 @@
         <v>18</v>
       </c>
       <c r="C2" s="4">
-        <f>B2/156</f>
+        <f t="shared" ref="C2:C47" si="0">B2/156</f>
         <v>0.11538461538461539</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F2" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -3353,95 +4194,119 @@
         <v>12</v>
       </c>
       <c r="C3" s="4">
-        <f>B3/156</f>
+        <f t="shared" si="0"/>
         <v>7.6923076923076927E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F3" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="B4">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="4">
-        <f>B4/156</f>
-        <v>7.0512820512820512E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v>6.4102564102564097E-2</v>
+      </c>
+      <c r="F4" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>7</v>
+      </c>
+      <c r="C5" s="4">
+        <f t="shared" si="0"/>
+        <v>4.4871794871794872E-2</v>
+      </c>
+      <c r="F5" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" s="4">
+        <f t="shared" si="0"/>
+        <v>3.2051282051282048E-2</v>
+      </c>
+      <c r="F6" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>10</v>
-      </c>
-      <c r="C5" s="4">
-        <f>B5/156</f>
-        <v>6.4102564102564097E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6">
-        <v>10</v>
-      </c>
-      <c r="C6" s="4">
-        <f>B6/156</f>
-        <v>6.4102564102564097E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7">
-        <v>10</v>
-      </c>
       <c r="C7" s="4">
-        <f>B7/156</f>
-        <v>6.4102564102564097E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v>2.564102564102564E-2</v>
+      </c>
+      <c r="F7" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B8">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C8" s="4">
-        <f>B8/156</f>
-        <v>6.4102564102564097E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v>1.282051282051282E-2</v>
+      </c>
+      <c r="F8" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B9">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C9" s="4">
-        <f>B9/156</f>
-        <v>5.128205128205128E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="F9" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="B10">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C10" s="4">
-        <f>B10/156</f>
-        <v>4.4871794871794872E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v>1.282051282051282E-2</v>
+      </c>
+      <c r="F10" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>53</v>
       </c>
@@ -3449,107 +4314,131 @@
         <v>6</v>
       </c>
       <c r="C11" s="4">
-        <f>B11/156</f>
+        <f t="shared" si="0"/>
         <v>3.8461538461538464E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F11" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>66</v>
       </c>
       <c r="B12">
         <v>5</v>
       </c>
       <c r="C12" s="4">
-        <f>B12/156</f>
+        <f t="shared" si="0"/>
         <v>3.2051282051282048E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F12" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>66</v>
+        <v>40</v>
       </c>
       <c r="B13">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C13" s="4">
-        <f>B13/156</f>
-        <v>3.2051282051282048E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="F13" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="B14">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C14" s="4">
-        <f>B14/156</f>
-        <v>2.564102564102564E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v>6.4102564102564097E-2</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="B15">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C15" s="4">
-        <f>B15/156</f>
-        <v>1.9230769230769232E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v>6.4102564102564097E-2</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="B16">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C16" s="4">
-        <f>B16/156</f>
-        <v>1.9230769230769232E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v>7.0512820512820512E-2</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B17">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C17" s="4">
-        <f>B17/156</f>
-        <v>1.282051282051282E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v>6.4102564102564097E-2</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18">
+        <v>8</v>
+      </c>
+      <c r="C18" s="4">
+        <f t="shared" si="0"/>
+        <v>5.128205128205128E-2</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
         <v>38</v>
-      </c>
-      <c r="B18">
-        <v>2</v>
-      </c>
-      <c r="C18" s="4">
-        <f>B18/156</f>
-        <v>1.282051282051282E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
-        <v>62</v>
       </c>
       <c r="B19">
         <v>2</v>
       </c>
       <c r="C19" s="4">
-        <f>B19/156</f>
+        <f t="shared" si="0"/>
         <v>1.282051282051282E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>33</v>
       </c>
@@ -3557,14 +4446,14 @@
         <v>1</v>
       </c>
       <c r="C20" s="4">
-        <f>B20/156</f>
+        <f t="shared" si="0"/>
         <v>6.41025641025641E-3</v>
       </c>
       <c r="D20" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>73</v>
       </c>
@@ -3572,11 +4461,14 @@
         <v>1</v>
       </c>
       <c r="C21" s="4">
-        <f>B21/156</f>
+        <f t="shared" si="0"/>
         <v>6.41025641025641E-3</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F21" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -3584,14 +4476,17 @@
         <v>1</v>
       </c>
       <c r="C22" s="4">
-        <f>B22/156</f>
+        <f t="shared" si="0"/>
         <v>6.41025641025641E-3</v>
       </c>
       <c r="D22" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F22" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -3599,14 +4494,17 @@
         <v>1</v>
       </c>
       <c r="C23" s="4">
-        <f>B23/156</f>
+        <f t="shared" si="0"/>
         <v>6.41025641025641E-3</v>
       </c>
       <c r="D23" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F23" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>39</v>
       </c>
@@ -3614,14 +4512,17 @@
         <v>1</v>
       </c>
       <c r="C24" s="4">
-        <f>B24/156</f>
+        <f t="shared" si="0"/>
         <v>6.41025641025641E-3</v>
       </c>
       <c r="D24" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F24" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>56</v>
       </c>
@@ -3629,11 +4530,11 @@
         <v>1</v>
       </c>
       <c r="C25" s="4">
-        <f>B25/156</f>
+        <f t="shared" si="0"/>
         <v>6.41025641025641E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>2</v>
       </c>
@@ -3641,14 +4542,14 @@
         <v>1</v>
       </c>
       <c r="C26" s="4">
-        <f>B26/156</f>
+        <f t="shared" si="0"/>
         <v>6.41025641025641E-3</v>
       </c>
       <c r="D26" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>37</v>
       </c>
@@ -3656,14 +4557,14 @@
         <v>1</v>
       </c>
       <c r="C27" s="4">
-        <f>B27/156</f>
+        <f t="shared" si="0"/>
         <v>6.41025641025641E-3</v>
       </c>
       <c r="D27" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>35</v>
       </c>
@@ -3671,11 +4572,11 @@
         <v>1</v>
       </c>
       <c r="C28" s="4">
-        <f>B28/156</f>
+        <f t="shared" si="0"/>
         <v>6.41025641025641E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>90</v>
       </c>
@@ -3683,11 +4584,11 @@
         <v>1</v>
       </c>
       <c r="C29" s="4">
-        <f>B29/156</f>
+        <f t="shared" si="0"/>
         <v>6.41025641025641E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>89</v>
       </c>
@@ -3695,11 +4596,11 @@
         <v>1</v>
       </c>
       <c r="C30" s="4">
-        <f>B30/156</f>
+        <f t="shared" si="0"/>
         <v>6.41025641025641E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>58</v>
       </c>
@@ -3707,14 +4608,14 @@
         <v>1</v>
       </c>
       <c r="C31" s="4">
-        <f>B31/156</f>
+        <f t="shared" si="0"/>
         <v>6.41025641025641E-3</v>
       </c>
       <c r="D31" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>71</v>
       </c>
@@ -3722,7 +4623,7 @@
         <v>1</v>
       </c>
       <c r="C32" s="4">
-        <f>B32/156</f>
+        <f t="shared" si="0"/>
         <v>6.41025641025641E-3</v>
       </c>
     </row>
@@ -3734,7 +4635,7 @@
         <v>1</v>
       </c>
       <c r="C33" s="4">
-        <f>B33/156</f>
+        <f t="shared" si="0"/>
         <v>6.41025641025641E-3</v>
       </c>
     </row>
@@ -3746,7 +4647,7 @@
         <v>1</v>
       </c>
       <c r="C34" s="4">
-        <f>B34/156</f>
+        <f t="shared" si="0"/>
         <v>6.41025641025641E-3</v>
       </c>
       <c r="D34" t="s">
@@ -3761,7 +4662,7 @@
         <v>1</v>
       </c>
       <c r="C35" s="4">
-        <f>B35/156</f>
+        <f t="shared" si="0"/>
         <v>6.41025641025641E-3</v>
       </c>
     </row>
@@ -3773,7 +4674,7 @@
         <v>1</v>
       </c>
       <c r="C36" s="4">
-        <f>B36/156</f>
+        <f t="shared" si="0"/>
         <v>6.41025641025641E-3</v>
       </c>
       <c r="E36" t="s">
@@ -3788,7 +4689,7 @@
         <v>1</v>
       </c>
       <c r="C37" s="4">
-        <f>B37/156</f>
+        <f t="shared" si="0"/>
         <v>6.41025641025641E-3</v>
       </c>
     </row>
@@ -3800,7 +4701,7 @@
         <v>1</v>
       </c>
       <c r="C38" s="4">
-        <f>B38/156</f>
+        <f t="shared" si="0"/>
         <v>6.41025641025641E-3</v>
       </c>
     </row>
@@ -3812,7 +4713,7 @@
         <v>1</v>
       </c>
       <c r="C39" s="4">
-        <f>B39/156</f>
+        <f t="shared" si="0"/>
         <v>6.41025641025641E-3</v>
       </c>
     </row>
@@ -3824,7 +4725,7 @@
         <v>1</v>
       </c>
       <c r="C40" s="4">
-        <f>B40/156</f>
+        <f t="shared" si="0"/>
         <v>6.41025641025641E-3</v>
       </c>
       <c r="D40" t="s">
@@ -3839,7 +4740,7 @@
         <v>1</v>
       </c>
       <c r="C41" s="4">
-        <f>B41/156</f>
+        <f t="shared" si="0"/>
         <v>6.41025641025641E-3</v>
       </c>
       <c r="D41" t="s">
@@ -3854,7 +4755,7 @@
         <v>1</v>
       </c>
       <c r="C42" s="4">
-        <f>B42/156</f>
+        <f t="shared" si="0"/>
         <v>6.41025641025641E-3</v>
       </c>
       <c r="D42" t="s">
@@ -3869,7 +4770,7 @@
         <v>1</v>
       </c>
       <c r="C43" s="4">
-        <f>B43/156</f>
+        <f t="shared" si="0"/>
         <v>6.41025641025641E-3</v>
       </c>
       <c r="D43" t="s">
@@ -3884,7 +4785,7 @@
         <v>1</v>
       </c>
       <c r="C44" s="4">
-        <f>B44/156</f>
+        <f t="shared" si="0"/>
         <v>6.41025641025641E-3</v>
       </c>
     </row>
@@ -3896,7 +4797,7 @@
         <v>1</v>
       </c>
       <c r="C45" s="4">
-        <f>B45/156</f>
+        <f t="shared" si="0"/>
         <v>6.41025641025641E-3</v>
       </c>
     </row>
@@ -3908,7 +4809,7 @@
         <v>1</v>
       </c>
       <c r="C46" s="4">
-        <f>B46/156</f>
+        <f t="shared" si="0"/>
         <v>6.41025641025641E-3</v>
       </c>
       <c r="E46" t="s">
@@ -3923,7 +4824,7 @@
         <v>1</v>
       </c>
       <c r="C47" s="4">
-        <f>B47/156</f>
+        <f t="shared" si="0"/>
         <v>6.41025641025641E-3</v>
       </c>
       <c r="D47" t="s">
@@ -3931,9 +4832,9 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E48" xr:uid="{BC4DB84E-5142-48A4-9DBD-FEBC42E0B80D}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E48">
-      <sortCondition descending="1" ref="B1:B48"/>
+  <autoFilter ref="A1:F47" xr:uid="{BC4DB84E-5142-48A4-9DBD-FEBC42E0B80D}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F47">
+      <sortCondition ref="F1:F47"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="C2:C47">

</xml_diff>